<commit_message>
New giant refactor and cleanup
</commit_message>
<xml_diff>
--- a/data/guns.xlsx
+++ b/data/guns.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23140" yWindow="5880" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="3920" yWindow="4220" windowWidth="19000" windowHeight="15160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="weapons.csv" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Shots</t>
-  </si>
-  <si>
     <t>ROF</t>
   </si>
   <si>
@@ -72,49 +69,52 @@
     <t>Snapfire: -2 to shots unless no movement this turn.</t>
   </si>
   <si>
-    <t>10mm</t>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>15/30/60</t>
+  </si>
+  <si>
+    <t>24/48/96</t>
+  </si>
+  <si>
+    <t>2d8</t>
+  </si>
+  <si>
+    <t>2d6+1</t>
+  </si>
+  <si>
+    <t>12/24/48</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Pipe Pistol</t>
+  </si>
+  <si>
+    <t>2d4</t>
+  </si>
+  <si>
+    <t>8/16/32</t>
+  </si>
+  <si>
+    <t>Cauterizing: +2 to Vigor tests to not bleed out.</t>
+  </si>
+  <si>
+    <t>10-mm</t>
   </si>
   <si>
     <t>.308</t>
   </si>
   <si>
-    <t>AP</t>
-  </si>
-  <si>
-    <t>15/30/60</t>
+    <t>.32</t>
+  </si>
+  <si>
+    <t>XShots</t>
   </si>
   <si>
     <t>Cell</t>
-  </si>
-  <si>
-    <t>24/48/96</t>
-  </si>
-  <si>
-    <t>2d8</t>
-  </si>
-  <si>
-    <t>2d6+1</t>
-  </si>
-  <si>
-    <t>12/24/48</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Pipe Pistol</t>
-  </si>
-  <si>
-    <t>2d4</t>
-  </si>
-  <si>
-    <t>8/16/32</t>
-  </si>
-  <si>
-    <t>.32</t>
-  </si>
-  <si>
-    <t>Cauterizing: +2 to Vigor tests to not bleed out.</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -531,34 +531,34 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -572,7 +572,7 @@
         <v>225</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
@@ -581,10 +581,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I2">
         <v>12</v>
@@ -616,10 +616,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I3">
         <v>30</v>
@@ -631,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -645,7 +645,7 @@
         <v>1500</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E4" s="4">
         <v>2</v>
@@ -654,10 +654,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -669,12 +669,12 @@
         <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
@@ -692,10 +692,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="I5">
         <v>12</v>
@@ -709,10 +709,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <ignoredErrors>
-    <ignoredError sqref="H4" numberStoredAsText="1"/>
-    <ignoredError sqref="G2" twoDigitTextYear="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Card resize and balance
</commit_message>
<xml_diff>
--- a/data/guns.xlsx
+++ b/data/guns.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Repos/savagewasteland/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B59DEC7-C495-534B-A19A-2356FA57A5DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924E3072-25D7-1449-B3F9-AB3159F2F4CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
     <sheet name="Boxes" sheetId="3" r:id="rId2"/>
     <sheet name="Mags" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -674,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,7 +735,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="6">
         <v>100</v>
@@ -770,7 +771,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3">
         <v>225</v>
@@ -806,7 +807,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3">
         <v>1500</v>
@@ -845,7 +846,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3">
         <v>30</v>
@@ -884,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3">
         <v>320</v>
@@ -919,7 +920,7 @@
         <v>44</v>
       </c>
       <c r="B8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3">
         <v>400</v>
@@ -954,7 +955,7 @@
         <v>45</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3">
         <v>800</v>
@@ -989,7 +990,7 @@
         <v>56</v>
       </c>
       <c r="B11" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3">
         <v>110</v>
@@ -1062,7 +1063,7 @@
         <v>49</v>
       </c>
       <c r="B14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3">
         <v>140</v>
@@ -1086,7 +1087,7 @@
         <v>6</v>
       </c>
       <c r="J14" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K14" t="s">
         <v>5</v>
@@ -1109,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1144,7 @@
         <v>33</v>
       </c>
       <c r="B2" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -1168,7 +1169,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -1193,7 +1194,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
         <v>4</v>
@@ -1218,7 +1219,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -1243,7 +1244,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
@@ -1293,7 +1294,7 @@
         <v>55</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3">
         <v>2</v>
@@ -1328,7 +1329,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1376,7 +1377,7 @@
         <v>9mm Pistol Mag</v>
       </c>
       <c r="C2" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>33</v>
@@ -1406,7 +1407,7 @@
         <v>10mm Pistol Mag</v>
       </c>
       <c r="C3" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>30</v>
@@ -1435,7 +1436,7 @@
         <v>Hunting Rifle Mag</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>27</v>
@@ -1496,7 +1497,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>26</v>
@@ -1520,7 +1521,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Post sesion 2 rebalance
</commit_message>
<xml_diff>
--- a/data/guns.xlsx
+++ b/data/guns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Repos/savagewasteland/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924E3072-25D7-1449-B3F9-AB3159F2F4CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E067CE3B-8EDA-EC48-BBA3-A0B071AF05AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -1110,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1328,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1407,7 +1407,7 @@
         <v>10mm Pistol Mag</v>
       </c>
       <c r="C3" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>30</v>
@@ -1465,7 +1465,7 @@
         <v>Pipe Pistol Mag</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>43</v>

</xml_diff>